<commit_message>
Expanded # of parameters and finished Tail Loop
See parameters.xlsx spreadsheet for details on what can be passed using the expanded variable list.
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="86">
   <si>
     <t>To send a message in a Linux terminal, run:</t>
   </si>
@@ -100,9 +100,6 @@
     <t>0-99%</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Red (0-255)</t>
   </si>
   <si>
@@ -146,10 +143,6 @@
   </si>
   <si>
     <t>Analog</t>
-  </si>
-  <si>
-    <t>Color from Wheel
-(0-360)</t>
   </si>
   <si>
     <t>Speed(2)</t>
@@ -225,22 +218,88 @@
     <t>(n*TailLength*numColors) + (col*TailLength)</t>
   </si>
   <si>
+    <t>0-99%(1)</t>
+  </si>
+  <si>
     <t>Color from Wheel
-(0-360) or
--1 for Random
--2 for Off</t>
-  </si>
-  <si>
-    <t>VarThree</t>
-  </si>
-  <si>
-    <t>VarFour</t>
-  </si>
-  <si>
-    <t>VarFive</t>
-  </si>
-  <si>
-    <t>VarSix</t>
+(0.0-360.0)
+-1-Random
+-2-Default/Red</t>
+  </si>
+  <si>
+    <t>Direction &amp; Fill:
+1 - Right, No Fill
+2 - Right, Fill Strip
+-1 - Left, No Fill
+-2 - Left, Fill Strip
+&gt;=3 - Fill, Alternate direction after X pixels</t>
+  </si>
+  <si>
+    <t>VarWheel[0]</t>
+  </si>
+  <si>
+    <t>VarWheel[1]</t>
+  </si>
+  <si>
+    <t>VarWheel[2]</t>
+  </si>
+  <si>
+    <t>VarWheel[3]</t>
+  </si>
+  <si>
+    <t>VarWheel[4]</t>
+  </si>
+  <si>
+    <t>[var3=]</t>
+  </si>
+  <si>
+    <t>[var4=]</t>
+  </si>
+  <si>
+    <t>[var5=]</t>
+  </si>
+  <si>
+    <t>[var6=]</t>
+  </si>
+  <si>
+    <t>[var7=]</t>
+  </si>
+  <si>
+    <t>N/A (-2.0)</t>
+  </si>
+  <si>
+    <t>N/A (0)</t>
+  </si>
+  <si>
+    <t>Length to Use
+0-Full Strip
+X-# of pixels wide</t>
+  </si>
+  <si>
+    <t>Centered Around Pixel
+-1 - Center of Strip
+X - Center on Pixel #X
+(ignored if VarOne = 0)</t>
+  </si>
+  <si>
+    <t>Color from Wheel
+(0.0-360.0)
+-1-Random
+-2-Random
+-3-White</t>
+  </si>
+  <si>
+    <t>Color from Wheel
+(0.0-360.0)
+-1-Random
+-2-Off
+-3-White</t>
+  </si>
+  <si>
+    <t>Christmas Example:</t>
+  </si>
+  <si>
+    <t>printf "?pin=1234&amp;effect=4&amp;var0=250&amp;var1=2&amp;var2=2&amp;var3=0&amp;var4=100&amp;var5=240&amp;var6=-3&amp;var7=25" | nc -u -q1 192.168.1.34 1337</t>
   </si>
 </sst>
 </file>
@@ -275,12 +334,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -295,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -342,10 +407,31 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -661,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
@@ -676,13 +762,14 @@
     <col min="7" max="7" width="12.54296875" style="4" customWidth="1"/>
     <col min="8" max="8" width="10.36328125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.81640625" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="2"/>
+    <col min="10" max="10" width="22.1796875" style="4" customWidth="1"/>
+    <col min="11" max="15" width="12.6328125" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="7"/>
@@ -695,18 +782,18 @@
       <c r="J1" s="7"/>
       <c r="K1" s="13"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="8"/>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="18" t="s">
-        <v>30</v>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
@@ -714,13 +801,13 @@
       <c r="J2" s="9"/>
       <c r="K2" s="13"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="18"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>6</v>
@@ -728,7 +815,7 @@
       <c r="E3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="18"/>
+      <c r="F3" s="19"/>
       <c r="G3" s="9" t="s">
         <v>8</v>
       </c>
@@ -741,43 +828,60 @@
       <c r="J3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="25" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="8"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="H4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="J4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="13"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K4" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="O4" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
@@ -800,17 +904,31 @@
         <v>25</v>
       </c>
       <c r="H5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="J5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="13"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K5" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>14</v>
       </c>
@@ -833,17 +951,31 @@
         <v>25</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>26</v>
+        <v>41</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>79</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="13"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="N6" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>18</v>
       </c>
@@ -866,17 +998,31 @@
         <v>25</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="13"/>
-    </row>
-    <row r="8" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
@@ -887,7 +1033,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>12</v>
@@ -895,21 +1041,35 @@
       <c r="F8" s="11">
         <v>3</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>26</v>
+      <c r="G8" s="21" t="s">
+        <v>65</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="13"/>
-    </row>
-    <row r="9" spans="1:14" ht="52.5" x14ac:dyDescent="0.25">
+      <c r="I8" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="K8" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="77.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>23</v>
       </c>
@@ -920,7 +1080,7 @@
         <v>22</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>12</v>
@@ -928,21 +1088,35 @@
       <c r="F9" s="11">
         <v>4</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>26</v>
+      <c r="G9" s="21" t="s">
+        <v>65</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="J9" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="K9" s="13"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K9" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="M9" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="N9" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="O9" s="23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
@@ -955,12 +1129,12 @@
       <c r="J10" s="7"/>
       <c r="K10" s="13"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -972,12 +1146,12 @@
       <c r="J11" s="7"/>
       <c r="K11" s="13"/>
     </row>
-    <row r="12" spans="1:14" ht="42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="42" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -989,7 +1163,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
@@ -1002,9 +1176,9 @@
       <c r="J13" s="7"/>
       <c r="K13" s="13"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
@@ -1017,9 +1191,9 @@
       <c r="J14" s="7"/>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
@@ -1032,9 +1206,9 @@
       <c r="J15" s="7"/>
       <c r="K15" s="13"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
@@ -1049,7 +1223,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
@@ -1064,7 +1238,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
@@ -1165,27 +1339,37 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1215,22 +1399,22 @@
   <sheetData>
     <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="S5" s="1">
         <f>30/(3*5)+1</f>
@@ -1239,12 +1423,12 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -1342,7 +1526,7 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -1440,7 +1624,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -1538,7 +1722,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B11" s="1">
         <f>B10*5*3+B9*5</f>

</xml_diff>

<commit_message>
Brightness controls added to CylonEye and Tail effects
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
   <si>
     <t>To send a message in a Linux terminal, run:</t>
   </si>
@@ -216,15 +216,6 @@
   </si>
   <si>
     <t>(n*TailLength*numColors) + (col*TailLength)</t>
-  </si>
-  <si>
-    <t>0-99%(1)</t>
-  </si>
-  <si>
-    <t>Color from Wheel
-(0.0-360.0)
--1-Random
--2-Default/Red</t>
   </si>
   <si>
     <t>Direction &amp; Fill:
@@ -276,12 +267,6 @@
 X-# of pixels wide</t>
   </si>
   <si>
-    <t>Centered Around Pixel
--1 - Center of Strip
-X - Center on Pixel #X
-(ignored if VarOne = 0)</t>
-  </si>
-  <si>
     <t>Color from Wheel
 (0.0-360.0)
 -1-Random
@@ -300,6 +285,19 @@
   </si>
   <si>
     <t>printf "?pin=1234&amp;effect=4&amp;var0=250&amp;var1=2&amp;var2=2&amp;var3=0&amp;var4=100&amp;var5=240&amp;var6=-3&amp;var7=25" | nc -u -q1 192.168.1.34 1337</t>
+  </si>
+  <si>
+    <t>Centered Around Pixel
+-1-Center of Strip
+X-Center on Pixel #X
+(ignored if VarOne = 0)</t>
+  </si>
+  <si>
+    <t>Color from Wheel
+(0.0-360.0)
+-1-Random
+-2-Default/Red
+-3-White</t>
   </si>
 </sst>
 </file>
@@ -360,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -406,6 +404,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -414,24 +427,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -749,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
@@ -783,16 +778,16 @@
       <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="8"/>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="19" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="24" t="s">
         <v>29</v>
       </c>
       <c r="G2" s="9"/>
@@ -802,7 +797,7 @@
       <c r="K2" s="13"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
@@ -815,7 +810,7 @@
       <c r="E3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="19"/>
+      <c r="F3" s="24"/>
       <c r="G3" s="9" t="s">
         <v>8</v>
       </c>
@@ -828,20 +823,20 @@
       <c r="J3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="N3" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="M3" s="25" t="s">
+      <c r="O3" s="21" t="s">
         <v>70</v>
-      </c>
-      <c r="N3" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="O3" s="25" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -866,19 +861,19 @@
         <v>34</v>
       </c>
       <c r="K4" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="M4" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="N4" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="O4" s="16" t="s">
         <v>75</v>
-      </c>
-      <c r="N4" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="O4" s="16" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -913,19 +908,19 @@
         <v>28</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -954,25 +949,25 @@
         <v>41</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1001,28 +996,28 @@
         <v>41</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N7" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="52.5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
@@ -1042,31 +1037,31 @@
         <v>3</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="J8" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="K8" s="23" t="s">
-        <v>66</v>
+      <c r="I8" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N8" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="77.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1089,7 +1084,7 @@
         <v>4</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>43</v>
@@ -1097,23 +1092,23 @@
       <c r="I9" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="J9" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="K9" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="L9" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="M9" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="N9" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="O9" s="23" t="s">
-        <v>83</v>
+      <c r="J9" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="L9" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="M9" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="O9" s="19" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1364,12 +1359,12 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Revised API and Flicker/Fire Effect
Review API.md for changes to the parameters.
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="88">
   <si>
     <t>To send a message in a Linux terminal, run:</t>
   </si>
@@ -297,6 +297,19 @@
 (0.0-360.0)
 -1-Random
 -2-Default/Red
+-3-White</t>
+  </si>
+  <si>
+    <t>Candle/Fireplace Flickering Effect</t>
+  </si>
+  <si>
+    <t>FLICKER</t>
+  </si>
+  <si>
+    <t>Color from Wheel
+(0.0-360.0)
+-1-Random
+-2-Default/Fire
 -3-White</t>
   </si>
 </sst>
@@ -358,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -417,6 +430,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -742,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
@@ -758,7 +774,8 @@
     <col min="8" max="8" width="10.36328125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.26953125" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.1796875" style="4" customWidth="1"/>
-    <col min="11" max="15" width="12.6328125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="13.36328125" style="2" customWidth="1"/>
+    <col min="12" max="15" width="12.6328125" style="2" customWidth="1"/>
     <col min="16" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
@@ -778,16 +795,16 @@
       <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="8"/>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="24" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="25" t="s">
         <v>29</v>
       </c>
       <c r="G2" s="9"/>
@@ -797,7 +814,7 @@
       <c r="K2" s="13"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
@@ -810,7 +827,7 @@
       <c r="E3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="24"/>
+      <c r="F3" s="25"/>
       <c r="G3" s="9" t="s">
         <v>8</v>
       </c>
@@ -1111,26 +1128,56 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="13"/>
+    <row r="10" spans="1:15" ht="68.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="22">
+        <v>5</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="N10" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="O10" s="22" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>37</v>
-      </c>
+      <c r="A11" s="7"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1141,12 +1188,12 @@
       <c r="J11" s="7"/>
       <c r="K11" s="13"/>
     </row>
-    <row r="12" spans="1:15" ht="42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -1158,9 +1205,13 @@
       <c r="J12" s="7"/>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="6"/>
+    <row r="13" spans="1:15" ht="42" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1172,9 +1223,7 @@
       <c r="K13" s="13"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>46</v>
-      </c>
+      <c r="A14" s="7"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -1188,7 +1237,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
@@ -1203,7 +1252,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
@@ -1218,7 +1267,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
@@ -1233,7 +1282,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
@@ -1247,7 +1296,9 @@
       <c r="K18" s="13"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
+      <c r="A19" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -1260,9 +1311,7 @@
       <c r="K19" s="13"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>0</v>
-      </c>
+      <c r="A20" s="10"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1275,8 +1324,8 @@
       <c r="K20" s="13"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>1</v>
+      <c r="A21" s="14" t="s">
+        <v>0</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
@@ -1290,7 +1339,9 @@
       <c r="K21" s="13"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
+      <c r="A22" s="15" t="s">
+        <v>1</v>
+      </c>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1303,9 +1354,7 @@
       <c r="K22" s="13"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
-        <v>2</v>
-      </c>
+      <c r="A23" s="10"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -1318,8 +1367,8 @@
       <c r="K23" s="13"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>3</v>
+      <c r="A24" s="14" t="s">
+        <v>2</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
@@ -1332,38 +1381,53 @@
       <c r="J24" s="7"/>
       <c r="K24" s="13"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>51</v>
-      </c>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="13"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>